<commit_message>
Added functioning to Player
</commit_message>
<xml_diff>
--- a/Data/CommonDialogs.xlsx
+++ b/Data/CommonDialogs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\Github\ProjectPyxis\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0594C3E-08E7-46CE-9C2C-E62D2036CAFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F7598AD-4F0A-433E-B591-492A5CEA6225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,16 +39,16 @@
     <t>room-enter</t>
   </si>
   <si>
-    <t>I have entered %roomname%</t>
-  </si>
-  <si>
-    <t>I am in the %roomname%</t>
-  </si>
-  <si>
     <t>game-start</t>
   </si>
   <si>
     <t>This is game start</t>
+  </si>
+  <si>
+    <t>I have entered {roomname}</t>
+  </si>
+  <si>
+    <t>I am in the {roomname}</t>
   </si>
 </sst>
 </file>
@@ -369,7 +369,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -400,7 +400,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -411,7 +411,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -419,10 +419,10 @@
         <v>600003</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed all basic functionality
</commit_message>
<xml_diff>
--- a/Data/CommonDialogs.xlsx
+++ b/Data/CommonDialogs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\Github\ProjectPyxis\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A038A5B7-3F1F-4869-9191-4094A35332CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6199D7D9-1F6E-42F1-94A5-905ADEDE4495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="73">
   <si>
     <t>DialogID</t>
   </si>
@@ -149,6 +148,102 @@
   </si>
   <si>
     <t>I currently do not have any items</t>
+  </si>
+  <si>
+    <t>room-active-node</t>
+  </si>
+  <si>
+    <t>room-inactive-node</t>
+  </si>
+  <si>
+    <t>There is a {nodename} which is working</t>
+  </si>
+  <si>
+    <t>There is a {nodename} which is not working</t>
+  </si>
+  <si>
+    <t>action-unable-rn</t>
+  </si>
+  <si>
+    <t>I am not able to perform that action right now</t>
+  </si>
+  <si>
+    <t>player-suicide-by-knife</t>
+  </si>
+  <si>
+    <t>I have stabbed myself.</t>
+  </si>
+  <si>
+    <t>game-end</t>
+  </si>
+  <si>
+    <t>Game ends.</t>
+  </si>
+  <si>
+    <t>npc-murdered-by-knife</t>
+  </si>
+  <si>
+    <t>{npcname} has stabbed himself.</t>
+  </si>
+  <si>
+    <t>player-escapes-pod</t>
+  </si>
+  <si>
+    <t>I have escaped the spacecraft via the escape pod.</t>
+  </si>
+  <si>
+    <t>player-suicide-by-gun</t>
+  </si>
+  <si>
+    <t>I have shot myself.</t>
+  </si>
+  <si>
+    <t>npc-murdered-by-gun</t>
+  </si>
+  <si>
+    <t>{npcname} is killed.</t>
+  </si>
+  <si>
+    <t>user-death-by-knife</t>
+  </si>
+  <si>
+    <t>{npcname} has stabbed me.</t>
+  </si>
+  <si>
+    <t>user-death-by-gun</t>
+  </si>
+  <si>
+    <t>{npcname} has shot me.</t>
+  </si>
+  <si>
+    <t>npc-death-by-knife</t>
+  </si>
+  <si>
+    <t>{npcname}  has stabbed himself.</t>
+  </si>
+  <si>
+    <t>npc-death-by-gun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{npcname}  has shot himself.  </t>
+  </si>
+  <si>
+    <t>npc-puts-batteries-pod</t>
+  </si>
+  <si>
+    <t>{npcname} has placed the batteries in escape pod.</t>
+  </si>
+  <si>
+    <t>npc-escapes-by-pod</t>
+  </si>
+  <si>
+    <t>{npcname} has escaped the spacecraft via the escape pod.</t>
+  </si>
+  <si>
+    <t>npc-in-room</t>
+  </si>
+  <si>
+    <t>{npcname} is here.</t>
   </si>
 </sst>
 </file>
@@ -184,7 +279,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -466,17 +562,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.21875" customWidth="1"/>
     <col min="2" max="2" width="40.33203125" customWidth="1"/>
-    <col min="3" max="3" width="40.21875" customWidth="1"/>
+    <col min="3" max="3" width="59.44140625" customWidth="1"/>
     <col min="4" max="4" width="44.88671875" customWidth="1"/>
     <col min="5" max="5" width="43.33203125" customWidth="1"/>
   </cols>
@@ -614,6 +710,9 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>600011</v>
+      </c>
       <c r="B13" t="s">
         <v>21</v>
       </c>
@@ -622,6 +721,9 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>600012</v>
+      </c>
       <c r="B14" t="s">
         <v>21</v>
       </c>
@@ -630,6 +732,9 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>600013</v>
+      </c>
       <c r="B15" t="s">
         <v>21</v>
       </c>
@@ -638,6 +743,9 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>600014</v>
+      </c>
       <c r="B16" t="s">
         <v>25</v>
       </c>
@@ -645,7 +753,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>600015</v>
+      </c>
       <c r="B17" t="s">
         <v>27</v>
       </c>
@@ -653,7 +764,10 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>600016</v>
+      </c>
       <c r="B18" t="s">
         <v>30</v>
       </c>
@@ -661,7 +775,10 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>600017</v>
+      </c>
       <c r="B19" t="s">
         <v>31</v>
       </c>
@@ -669,7 +786,10 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>600018</v>
+      </c>
       <c r="B20" t="s">
         <v>33</v>
       </c>
@@ -677,7 +797,10 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>600019</v>
+      </c>
       <c r="B21" t="s">
         <v>35</v>
       </c>
@@ -685,7 +808,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>600020</v>
+      </c>
       <c r="B22" t="s">
         <v>37</v>
       </c>
@@ -693,12 +819,191 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>600021</v>
+      </c>
       <c r="B23" t="s">
         <v>38</v>
       </c>
       <c r="C23" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>600022</v>
+      </c>
+      <c r="B24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>600023</v>
+      </c>
+      <c r="B25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>600024</v>
+      </c>
+      <c r="B26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>600025</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>600026</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>600027</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>600028</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>600029</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>600030</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>600031</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>600032</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>600033</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>600034</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>600035</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>600036</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>600037</v>
+      </c>
+      <c r="B39" t="s">
+        <v>71</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>